<commit_message>
Updated figures and needed files
</commit_message>
<xml_diff>
--- a/Results/Lm_SAR_Results.xlsx
+++ b/Results/Lm_SAR_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Friederike\Documents\GitHub\FruitsAfrica\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFE9B06-5815-44C0-B589-9CEC6DB0486F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14106F45-CF63-493F-9A67-3603183B8B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="13223" xr2:uid="{933A1E10-8C6C-4D91-BC76-9ECD2451CDAE}"/>
+    <workbookView xWindow="7020" yWindow="2213" windowWidth="21600" windowHeight="13222" xr2:uid="{933A1E10-8C6C-4D91-BC76-9ECD2451CDAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="114">
   <si>
     <t>Call:</t>
   </si>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>p-value</t>
-  </si>
-  <si>
-    <t>&lt; 2.2e-16</t>
   </si>
   <si>
     <t xml:space="preserve">Moran I statistic standard deviate </t>
@@ -468,12 +465,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -484,6 +499,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E20CCA4-D63A-46CB-84F8-69BA8ADB9C18}" name="Table1" displayName="Table1" ref="A107:F110" totalsRowShown="0">
+  <autoFilter ref="A107:F110" xr:uid="{5E20CCA4-D63A-46CB-84F8-69BA8ADB9C18}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{50EBB261-480B-4A4A-BB70-9CC1951E4FE0}" name="Moran I statistic"/>
+    <tableColumn id="2" xr3:uid="{547DE2FC-8C20-4729-BC31-1621FA4F3EA2}" name="Expectation" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{24136489-E5E0-4CCA-9CDD-C92201BA43B0}" name="Variance" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{29A2EFF7-FC00-49C3-948E-AD096CA21F0E}" name="data" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{91C31BD8-5BF5-4644-BE8D-80C261F4D211}" name="Moran I statistic standard deviate " dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{8F107F81-FB36-4579-A500-2F7B5986320B}" name="p-value" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -785,13 +815,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AEBEE6-A5BD-4D33-B188-53E40F35F757}">
   <dimension ref="A1:R110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="49" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="9.3984375" customWidth="1"/>
+    <col min="5" max="5" width="29.53125" customWidth="1"/>
     <col min="11" max="11" width="9.06640625" style="7"/>
     <col min="12" max="12" width="23.06640625" customWidth="1"/>
   </cols>
@@ -2423,91 +2456,94 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B107" t="s">
+        <v>106</v>
+      </c>
+      <c r="C107" t="s">
         <v>107</v>
       </c>
-      <c r="C107" t="s">
-        <v>108</v>
-      </c>
       <c r="D107" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F107" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A108" s="3">
+      <c r="A108" s="11">
         <v>0.73600849400000001</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="9">
         <v>-8.5470089999999995E-3</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="4">
         <v>3.6754489999999999E-3</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E108" s="4">
+        <v>12.281000000000001</v>
+      </c>
+      <c r="F108" s="8">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A109" s="4">
+        <v>0.265804188</v>
+      </c>
+      <c r="B109" s="9">
+        <v>-8.5470089999999995E-3</v>
+      </c>
+      <c r="C109" s="4">
+        <v>3.6186370000000001E-3</v>
+      </c>
+      <c r="D109" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E108">
-        <v>12.281000000000001</v>
-      </c>
-      <c r="F108" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A109">
-        <v>0.265804188</v>
-      </c>
-      <c r="B109">
+      <c r="E109" s="4">
+        <v>4.5606999999999998</v>
+      </c>
+      <c r="F109" s="8">
+        <v>5.0980000000000001E-6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A110" s="4">
+        <v>0.14843287799999999</v>
+      </c>
+      <c r="B110" s="9">
         <v>-8.5470089999999995E-3</v>
       </c>
-      <c r="C109">
-        <v>3.6186370000000001E-3</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C110" s="4">
+        <v>3.6179269999999999E-3</v>
+      </c>
+      <c r="D110" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E109">
-        <v>4.5606999999999998</v>
-      </c>
-      <c r="F109" s="11">
-        <v>5.0980000000000001E-6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A110">
-        <v>0.14843287799999999</v>
-      </c>
-      <c r="B110">
-        <v>-8.5470089999999995E-3</v>
-      </c>
-      <c r="C110">
-        <v>3.6179269999999999E-3</v>
-      </c>
-      <c r="D110" t="s">
-        <v>112</v>
-      </c>
-      <c r="E110">
+      <c r="E110" s="4">
         <v>2.6097999999999999</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="8">
         <v>9.0580000000000001E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>